<commit_message>
Update README for environment setup and add Docker build workflow
- Corrected the commands in the README for copying the example environment file.
- Introduced a new GitHub Actions workflow for Docker build testing, which includes steps to copy the environment file and build Docker services.
- Updated the binary file 'lilly_data.xlsx' in the uploads directory.
</commit_message>
<xml_diff>
--- a/uploads/lilly_data.xlsx
+++ b/uploads/lilly_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/GitHub/carin-db/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F044B-7614-3A4D-AE89-AF833C3A05AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF923A1-9607-7845-BB50-892AFB1A9F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="-28300" windowWidth="34400" windowHeight="28300" tabRatio="764" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19340" yWindow="-28300" windowWidth="68800" windowHeight="28300" tabRatio="764" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Molecule" sheetId="56" r:id="rId1"/>
@@ -943,13 +943,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,7 +1241,7 @@
   <dimension ref="A1:BG54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1270,13 +1270,13 @@
       <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="8"/>
@@ -1755,7 +1755,7 @@
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="20" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
@@ -2132,7 +2132,7 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -2191,7 +2191,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>149</v>
       </c>
       <c r="G2" s="1">
@@ -2261,7 +2261,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2349,7 +2349,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>155</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2701,7 +2701,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>161</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2789,7 +2789,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>163</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2877,7 +2877,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>165</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2953,7 +2953,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>167</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3029,7 +3029,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>169</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -3187,7 +3187,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>173</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3202,7 +3202,7 @@
       <c r="E26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G26" s="1">
@@ -3246,7 +3246,7 @@
       <c r="E27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="27" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1">
@@ -3287,8 +3287,8 @@
   </sheetPr>
   <dimension ref="A1:Q253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15623,7 +15623,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>151</v>
       </c>

</xml_diff>